<commit_message>
latest version showing testing of RML load
</commit_message>
<xml_diff>
--- a/data/metrics_data-compare.xlsx
+++ b/data/metrics_data-compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06d335bcba30d7c9/MSc Data Science my assignments/10 Individual Project/iteration3/git-repo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{64AC38A9-2F7C-48E1-9E63-848BF6AFEB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EEA43EE-2E37-4600-AF68-B79F2215E5FA}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{64AC38A9-2F7C-48E1-9E63-848BF6AFEB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F730BE0E-908E-42C7-AAB0-42BDDA644736}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="56">
   <si>
     <t>Original Test Input Data</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Manufacturer</t>
   </si>
   <si>
-    <t>P135</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -103,27 +100,9 @@
     <t>Siemens</t>
   </si>
   <si>
-    <t>P272</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>P273</t>
-  </si>
-  <si>
-    <t>P274</t>
-  </si>
-  <si>
-    <t>P275</t>
-  </si>
-  <si>
-    <t>P276</t>
-  </si>
-  <si>
-    <t>P277</t>
-  </si>
-  <si>
     <t>P005</t>
   </si>
   <si>
@@ -133,21 +112,6 @@
     <t>Philips</t>
   </si>
   <si>
-    <t>P278</t>
-  </si>
-  <si>
-    <t>P279</t>
-  </si>
-  <si>
-    <t>P280</t>
-  </si>
-  <si>
-    <t>P281</t>
-  </si>
-  <si>
-    <t>P282</t>
-  </si>
-  <si>
     <t>Siemens_ModelA</t>
   </si>
   <si>
@@ -155,6 +119,87 @@
   </si>
   <si>
     <t>Paste in metric_data.csv (Original Test Input Data) and metrics_data_replicate (Replicated data) and check that compare results all 'match'</t>
+  </si>
+  <si>
+    <t>P935</t>
+  </si>
+  <si>
+    <t>P973</t>
+  </si>
+  <si>
+    <t>P974</t>
+  </si>
+  <si>
+    <t>Siemens_ModelB</t>
+  </si>
+  <si>
+    <t>P975</t>
+  </si>
+  <si>
+    <t>P976</t>
+  </si>
+  <si>
+    <t>P977</t>
+  </si>
+  <si>
+    <t>P978</t>
+  </si>
+  <si>
+    <t>P979</t>
+  </si>
+  <si>
+    <t>P980</t>
+  </si>
+  <si>
+    <t>Philips_ModelB</t>
+  </si>
+  <si>
+    <t>P981</t>
+  </si>
+  <si>
+    <t>P989</t>
+  </si>
+  <si>
+    <t>P005/2</t>
+  </si>
+  <si>
+    <t>P935/1</t>
+  </si>
+  <si>
+    <t>P973/1</t>
+  </si>
+  <si>
+    <t>P974/1</t>
+  </si>
+  <si>
+    <t>P975/1</t>
+  </si>
+  <si>
+    <t>P976/1</t>
+  </si>
+  <si>
+    <t>P977/1</t>
+  </si>
+  <si>
+    <t>P978/2</t>
+  </si>
+  <si>
+    <t>P979/2</t>
+  </si>
+  <si>
+    <t>P980/2</t>
+  </si>
+  <si>
+    <t>P981/2</t>
+  </si>
+  <si>
+    <t>P989/2</t>
+  </si>
+  <si>
+    <t>P979/1</t>
+  </si>
+  <si>
+    <t>concat in KG</t>
   </si>
 </sst>
 </file>
@@ -660,13 +705,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1022,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI15"/>
+  <dimension ref="A1:AI16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="W3" sqref="W3:X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,74 +1095,74 @@
       </c>
     </row>
     <row r="2" spans="1:35" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="2"/>
-      <c r="M2" s="4" t="s">
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" t="s">
         <v>16</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" t="s">
         <v>18</v>
       </c>
       <c r="Y2" s="2"/>
@@ -1153,81 +1199,78 @@
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
+      <c r="E3">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>22</v>
-      </c>
       <c r="F3">
-        <v>712</v>
+        <v>799</v>
       </c>
       <c r="G3">
-        <v>5.7</v>
+        <v>6.3</v>
       </c>
       <c r="H3">
-        <v>24.2</v>
+        <v>32.4</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="J3">
         <v>1.5</v>
       </c>
-      <c r="K3">
-        <v>998</v>
-      </c>
       <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3">
+        <v>58</v>
+      </c>
+      <c r="P3" t="s">
         <v>19</v>
       </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
+      <c r="Q3">
         <v>25</v>
       </c>
-      <c r="P3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3">
-        <v>22</v>
-      </c>
       <c r="R3">
-        <v>712</v>
+        <v>799</v>
       </c>
       <c r="S3">
-        <v>5.7</v>
+        <v>6.3</v>
       </c>
       <c r="T3">
-        <v>24.2</v>
+        <v>32.4</v>
       </c>
       <c r="U3" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="V3">
         <v>1.5</v>
       </c>
-      <c r="W3" t="s">
-        <v>21</v>
-      </c>
-      <c r="X3" t="s">
-        <v>22</v>
+      <c r="W3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="Z3" t="str">
         <f>IF(A3=M3,"match","error")</f>
         <v>match</v>
       </c>
-      <c r="AA3" t="str">
-        <f t="shared" ref="AA3:AI15" si="0">IF(B3=N3,"match","error")</f>
-        <v>match</v>
+      <c r="AA3" s="5" t="str">
+        <f t="shared" ref="AA3:AI9" si="0">IF(B3=N3,"match","error")</f>
+        <v>error</v>
       </c>
       <c r="AB3" t="str">
         <f t="shared" si="0"/>
@@ -1264,81 +1307,78 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E4">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F4">
-        <v>789</v>
+        <v>712</v>
       </c>
       <c r="G4">
-        <v>9.1999999999999993</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H4">
-        <v>27.5</v>
+        <v>24.2</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J4">
         <v>1.5</v>
       </c>
-      <c r="K4">
-        <v>999</v>
-      </c>
       <c r="M4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
+        <v>43</v>
       </c>
       <c r="O4">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="P4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="Q4">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="R4">
-        <v>789</v>
+        <v>712</v>
       </c>
       <c r="S4">
-        <v>9.1999999999999993</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="T4">
-        <v>27.5</v>
+        <v>24.2</v>
       </c>
       <c r="U4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="V4">
         <v>1.5</v>
       </c>
-      <c r="W4" t="s">
+      <c r="W4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="X4" t="s">
-        <v>22</v>
-      </c>
       <c r="Z4" t="str">
-        <f t="shared" ref="Z4:Z15" si="1">IF(A4=M4,"match","error")</f>
-        <v>match</v>
-      </c>
-      <c r="AA4" t="str">
-        <f t="shared" si="0"/>
-        <v>match</v>
+        <f t="shared" ref="Z4:Z9" si="1">IF(A4=M4,"match","error")</f>
+        <v>match</v>
+      </c>
+      <c r="AA4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>error</v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="0"/>
@@ -1375,7 +1415,7 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1384,7 +1424,7 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>28</v>
@@ -1399,25 +1439,22 @@
         <v>30.8</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J5">
         <v>1.5</v>
       </c>
-      <c r="K5">
-        <v>1000</v>
-      </c>
       <c r="M5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>44</v>
       </c>
       <c r="O5">
         <v>38</v>
       </c>
       <c r="P5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q5">
         <v>28</v>
@@ -1432,24 +1469,24 @@
         <v>30.8</v>
       </c>
       <c r="U5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="V5">
         <v>1.5</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X5" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="X5" t="s">
-        <v>22</v>
       </c>
       <c r="Z5" t="str">
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="AA5" t="str">
-        <f t="shared" si="0"/>
-        <v>match</v>
+      <c r="AA5" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>error</v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="0"/>
@@ -1486,7 +1523,7 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1495,7 +1532,7 @@
         <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>29.5</v>
@@ -1510,25 +1547,22 @@
         <v>34.1</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J6">
-        <v>1.5</v>
-      </c>
-      <c r="K6">
-        <v>1001</v>
+        <v>3</v>
       </c>
       <c r="M6" t="s">
-        <v>26</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="N6" t="s">
+        <v>45</v>
       </c>
       <c r="O6">
         <v>39</v>
       </c>
       <c r="P6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q6">
         <v>29.5</v>
@@ -1543,24 +1577,24 @@
         <v>34.1</v>
       </c>
       <c r="U6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="V6">
-        <v>1.5</v>
-      </c>
-      <c r="W6" t="s">
+        <v>3</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X6" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="X6" t="s">
-        <v>22</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="AA6" t="str">
-        <f t="shared" si="0"/>
-        <v>match</v>
+      <c r="AA6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>error</v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="0"/>
@@ -1597,7 +1631,7 @@
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1606,7 +1640,7 @@
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <v>31</v>
@@ -1621,25 +1655,22 @@
         <v>37.4</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J7">
-        <v>1.5</v>
-      </c>
-      <c r="K7">
-        <v>1002</v>
+        <v>3</v>
       </c>
       <c r="M7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="N7" t="s">
+        <v>46</v>
       </c>
       <c r="O7">
         <v>40</v>
       </c>
       <c r="P7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q7">
         <v>31</v>
@@ -1654,24 +1685,24 @@
         <v>37.4</v>
       </c>
       <c r="U7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="V7">
-        <v>1.5</v>
-      </c>
-      <c r="W7" t="s">
+        <v>3</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X7" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="X7" t="s">
-        <v>22</v>
       </c>
       <c r="Z7" t="str">
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="AA7" t="str">
-        <f t="shared" si="0"/>
-        <v>match</v>
+      <c r="AA7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>error</v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="0"/>
@@ -1708,7 +1739,7 @@
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1717,7 +1748,7 @@
         <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8">
         <v>32.5</v>
@@ -1732,25 +1763,22 @@
         <v>40.700000000000003</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J8">
-        <v>1.5</v>
-      </c>
-      <c r="K8">
-        <v>1003</v>
+        <v>3</v>
       </c>
       <c r="M8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="N8" t="s">
+        <v>47</v>
       </c>
       <c r="O8">
         <v>41</v>
       </c>
       <c r="P8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q8">
         <v>32.5</v>
@@ -1765,24 +1793,24 @@
         <v>40.700000000000003</v>
       </c>
       <c r="U8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="V8">
-        <v>1.5</v>
-      </c>
-      <c r="W8" t="s">
+        <v>3</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X8" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="X8" t="s">
-        <v>22</v>
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="AA8" t="str">
-        <f t="shared" si="0"/>
-        <v>match</v>
+      <c r="AA8" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>error</v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="0"/>
@@ -1819,7 +1847,7 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1828,7 +1856,7 @@
         <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9">
         <v>34</v>
@@ -1843,25 +1871,22 @@
         <v>44</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J9">
-        <v>1.5</v>
-      </c>
-      <c r="K9">
-        <v>1004</v>
+        <v>3</v>
       </c>
       <c r="M9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="N9" t="s">
+        <v>48</v>
       </c>
       <c r="O9">
         <v>42</v>
       </c>
       <c r="P9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q9">
         <v>34</v>
@@ -1876,24 +1901,24 @@
         <v>44</v>
       </c>
       <c r="U9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="V9">
-        <v>1.5</v>
-      </c>
-      <c r="W9" t="s">
+        <v>3</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X9" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="X9" t="s">
-        <v>22</v>
       </c>
       <c r="Z9" t="str">
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="AA9" t="str">
-        <f t="shared" si="0"/>
-        <v>match</v>
+      <c r="AA9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>error</v>
       </c>
       <c r="AB9" t="str">
         <f t="shared" si="0"/>
@@ -1930,229 +1955,223 @@
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E10">
-        <v>25</v>
+        <v>35.5</v>
       </c>
       <c r="F10">
-        <v>803</v>
+        <v>837</v>
       </c>
       <c r="G10">
-        <v>6.3</v>
+        <v>12.2</v>
       </c>
       <c r="H10">
-        <v>32.4</v>
+        <v>47.3</v>
       </c>
       <c r="I10" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="J10">
         <v>1.5</v>
       </c>
-      <c r="K10">
-        <v>997</v>
-      </c>
       <c r="M10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10">
-        <v>2</v>
+        <v>36</v>
+      </c>
+      <c r="N10" t="s">
+        <v>49</v>
       </c>
       <c r="O10">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="P10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q10">
-        <v>25</v>
+        <v>35.5</v>
       </c>
       <c r="R10">
-        <v>803</v>
+        <v>837</v>
       </c>
       <c r="S10">
-        <v>6.3</v>
+        <v>12.2</v>
       </c>
       <c r="T10">
-        <v>32.4</v>
+        <v>47.3</v>
       </c>
       <c r="U10" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="V10">
         <v>1.5</v>
       </c>
-      <c r="W10" t="s">
-        <v>21</v>
-      </c>
-      <c r="X10" t="s">
-        <v>32</v>
+      <c r="W10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X10" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="Z10" t="str">
-        <f t="shared" si="1"/>
-        <v>match</v>
-      </c>
-      <c r="AA10" t="str">
-        <f t="shared" si="0"/>
-        <v>match</v>
+        <f t="shared" ref="Z10:Z15" si="2">IF(A10=M10,"match","error")</f>
+        <v>match</v>
+      </c>
+      <c r="AA10" s="5" t="str">
+        <f t="shared" ref="AA10:AA15" si="3">IF(B10=N10,"match","error")</f>
+        <v>error</v>
       </c>
       <c r="AB10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AB10:AB15" si="4">IF(C10=O10,"match","error")</f>
         <v>match</v>
       </c>
       <c r="AC10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AC10:AC15" si="5">IF(D10=P10,"match","error")</f>
         <v>match</v>
       </c>
       <c r="AD10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AD10:AD15" si="6">IF(E10=Q10,"match","error")</f>
         <v>match</v>
       </c>
       <c r="AE10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AE10:AE15" si="7">IF(F10=R10,"match","error")</f>
         <v>match</v>
       </c>
       <c r="AF10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AF10:AF15" si="8">IF(G10=S10,"match","error")</f>
         <v>match</v>
       </c>
       <c r="AG10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AG10:AG15" si="9">IF(H10=T10,"match","error")</f>
         <v>match</v>
       </c>
       <c r="AH10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AH10:AH15" si="10">IF(I10=U10,"match","error")</f>
         <v>match</v>
       </c>
       <c r="AI10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AI10:AI15" si="11">IF(J10=V10,"match","error")</f>
         <v>match</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E11">
-        <v>35.5</v>
+        <v>37</v>
       </c>
       <c r="F11">
-        <v>837</v>
+        <v>789</v>
       </c>
       <c r="G11">
-        <v>2.2000000000000002</v>
+        <v>6</v>
       </c>
       <c r="H11">
-        <v>47.3</v>
+        <v>27.5</v>
       </c>
       <c r="I11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J11">
         <v>1.5</v>
       </c>
-      <c r="K11">
-        <v>1005</v>
-      </c>
       <c r="M11" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11">
-        <v>2</v>
+        <v>37</v>
+      </c>
+      <c r="N11" t="s">
+        <v>54</v>
       </c>
       <c r="O11">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="Q11">
-        <v>35.5</v>
+        <v>37</v>
       </c>
       <c r="R11">
-        <v>837</v>
+        <v>789</v>
       </c>
       <c r="S11">
-        <v>2.2000000000000002</v>
+        <v>6</v>
       </c>
       <c r="T11">
-        <v>47.3</v>
+        <v>27.5</v>
       </c>
       <c r="U11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="V11">
         <v>1.5</v>
       </c>
-      <c r="W11" t="s">
+      <c r="W11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="X11" t="s">
-        <v>32</v>
-      </c>
       <c r="Z11" t="str">
-        <f t="shared" si="1"/>
-        <v>match</v>
-      </c>
-      <c r="AA11" t="str">
-        <f t="shared" si="0"/>
-        <v>match</v>
+        <f t="shared" si="2"/>
+        <v>match</v>
+      </c>
+      <c r="AA11" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>error</v>
       </c>
       <c r="AB11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>match</v>
       </c>
       <c r="AC11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>match</v>
       </c>
       <c r="AD11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>match</v>
       </c>
       <c r="AE11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>match</v>
       </c>
       <c r="AF11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>match</v>
       </c>
       <c r="AG11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>match</v>
       </c>
       <c r="AH11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>match</v>
       </c>
       <c r="AI11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>match</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -2161,7 +2180,7 @@
         <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12">
         <v>37</v>
@@ -2170,31 +2189,28 @@
         <v>846</v>
       </c>
       <c r="G12">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="H12">
         <v>50.6</v>
       </c>
       <c r="I12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="J12">
         <v>1.5</v>
       </c>
-      <c r="K12">
-        <v>1006</v>
-      </c>
       <c r="M12" t="s">
-        <v>34</v>
-      </c>
-      <c r="N12">
-        <v>2</v>
+        <v>37</v>
+      </c>
+      <c r="N12" t="s">
+        <v>50</v>
       </c>
       <c r="O12">
         <v>44</v>
       </c>
       <c r="P12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q12">
         <v>37</v>
@@ -2203,67 +2219,67 @@
         <v>846</v>
       </c>
       <c r="S12">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="T12">
         <v>50.6</v>
       </c>
       <c r="U12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="V12">
         <v>1.5</v>
       </c>
-      <c r="W12" t="s">
-        <v>21</v>
-      </c>
-      <c r="X12" t="s">
-        <v>32</v>
+      <c r="W12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X12" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="Z12" t="str">
-        <f t="shared" si="1"/>
-        <v>match</v>
-      </c>
-      <c r="AA12" t="str">
-        <f t="shared" si="0"/>
-        <v>match</v>
+        <f t="shared" si="2"/>
+        <v>match</v>
+      </c>
+      <c r="AA12" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>error</v>
       </c>
       <c r="AB12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>match</v>
       </c>
       <c r="AC12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>match</v>
       </c>
       <c r="AD12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>match</v>
       </c>
       <c r="AE12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>match</v>
       </c>
       <c r="AF12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>match</v>
       </c>
       <c r="AG12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>match</v>
       </c>
       <c r="AH12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>match</v>
       </c>
       <c r="AI12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>match</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -2272,13 +2288,13 @@
         <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13">
         <v>38.5</v>
       </c>
       <c r="F13">
-        <v>855</v>
+        <v>788</v>
       </c>
       <c r="G13">
         <v>12</v>
@@ -2287,31 +2303,28 @@
         <v>53.9</v>
       </c>
       <c r="I13" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="J13">
-        <v>1.5</v>
-      </c>
-      <c r="K13">
-        <v>1007</v>
+        <v>5</v>
       </c>
       <c r="M13" t="s">
-        <v>35</v>
-      </c>
-      <c r="N13">
-        <v>2</v>
+        <v>38</v>
+      </c>
+      <c r="N13" t="s">
+        <v>51</v>
       </c>
       <c r="O13">
         <v>45</v>
       </c>
       <c r="P13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q13">
         <v>38.5</v>
       </c>
       <c r="R13">
-        <v>855</v>
+        <v>788</v>
       </c>
       <c r="S13">
         <v>12</v>
@@ -2320,61 +2333,61 @@
         <v>53.9</v>
       </c>
       <c r="U13" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="V13">
-        <v>1.5</v>
-      </c>
-      <c r="W13" t="s">
-        <v>21</v>
-      </c>
-      <c r="X13" t="s">
-        <v>32</v>
+        <v>5</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X13" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="Z13" t="str">
-        <f t="shared" si="1"/>
-        <v>match</v>
-      </c>
-      <c r="AA13" t="str">
-        <f t="shared" si="0"/>
-        <v>match</v>
+        <f t="shared" si="2"/>
+        <v>match</v>
+      </c>
+      <c r="AA13" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>error</v>
       </c>
       <c r="AB13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>match</v>
       </c>
       <c r="AC13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>match</v>
       </c>
       <c r="AD13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>match</v>
       </c>
       <c r="AE13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>match</v>
       </c>
       <c r="AF13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>match</v>
       </c>
       <c r="AG13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>match</v>
       </c>
       <c r="AH13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>match</v>
       </c>
       <c r="AI13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>match</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -2383,7 +2396,7 @@
         <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14">
         <v>40</v>
@@ -2398,25 +2411,22 @@
         <v>57.2</v>
       </c>
       <c r="I14" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="J14">
-        <v>1.5</v>
-      </c>
-      <c r="K14">
-        <v>1008</v>
+        <v>5</v>
       </c>
       <c r="M14" t="s">
-        <v>36</v>
-      </c>
-      <c r="N14">
-        <v>2</v>
+        <v>40</v>
+      </c>
+      <c r="N14" t="s">
+        <v>52</v>
       </c>
       <c r="O14">
         <v>46</v>
       </c>
       <c r="P14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q14">
         <v>40</v>
@@ -2431,61 +2441,61 @@
         <v>57.2</v>
       </c>
       <c r="U14" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="V14">
-        <v>1.5</v>
-      </c>
-      <c r="W14" t="s">
-        <v>21</v>
-      </c>
-      <c r="X14" t="s">
-        <v>32</v>
+        <v>5</v>
+      </c>
+      <c r="W14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X14" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="Z14" t="str">
-        <f t="shared" si="1"/>
-        <v>match</v>
-      </c>
-      <c r="AA14" t="str">
-        <f t="shared" si="0"/>
-        <v>match</v>
+        <f t="shared" si="2"/>
+        <v>match</v>
+      </c>
+      <c r="AA14" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>error</v>
       </c>
       <c r="AB14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>match</v>
       </c>
       <c r="AC14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>match</v>
       </c>
       <c r="AD14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>match</v>
       </c>
       <c r="AE14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>match</v>
       </c>
       <c r="AF14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>match</v>
       </c>
       <c r="AG14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>match</v>
       </c>
       <c r="AH14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>match</v>
       </c>
       <c r="AI14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>match</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -2494,7 +2504,7 @@
         <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15">
         <v>41.5</v>
@@ -2509,25 +2519,22 @@
         <v>60.5</v>
       </c>
       <c r="I15" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="J15">
-        <v>1.5</v>
-      </c>
-      <c r="K15">
-        <v>1009</v>
+        <v>5</v>
       </c>
       <c r="M15" t="s">
-        <v>37</v>
-      </c>
-      <c r="N15">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="N15" t="s">
+        <v>53</v>
       </c>
       <c r="O15">
         <v>47</v>
       </c>
       <c r="P15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q15">
         <v>41.5</v>
@@ -2542,56 +2549,61 @@
         <v>60.5</v>
       </c>
       <c r="U15" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="V15">
-        <v>1.5</v>
-      </c>
-      <c r="W15" t="s">
-        <v>21</v>
-      </c>
-      <c r="X15" t="s">
-        <v>32</v>
+        <v>5</v>
+      </c>
+      <c r="W15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X15" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="Z15" t="str">
-        <f t="shared" si="1"/>
-        <v>match</v>
-      </c>
-      <c r="AA15" t="str">
-        <f t="shared" si="0"/>
-        <v>match</v>
+        <f t="shared" si="2"/>
+        <v>match</v>
+      </c>
+      <c r="AA15" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>error</v>
       </c>
       <c r="AB15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>match</v>
       </c>
       <c r="AC15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>match</v>
       </c>
       <c r="AD15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>match</v>
       </c>
       <c r="AE15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>match</v>
       </c>
       <c r="AF15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>match</v>
       </c>
       <c r="AG15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>match</v>
       </c>
       <c r="AH15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>match</v>
       </c>
       <c r="AI15" t="str">
-        <f t="shared" si="0"/>
-        <v>match</v>
+        <f t="shared" si="11"/>
+        <v>match</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AA16" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2613,14 +2625,14 @@
     <col min="1" max="1" width="125.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>39</v>
+    <row r="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>40</v>
+    <row r="2" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>